<commit_message>
Updated PMF/PDF formulae, mean/variance for some distributions
</commit_message>
<xml_diff>
--- a/probability_distributions_cheat_sheet.xlsx
+++ b/probability_distributions_cheat_sheet.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syerrapr/Documents/personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syerrapr/Documents/personal/cheat-sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA3463C-B6AF-1D4A-BFFE-41B917080915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C824AD07-BA0A-5343-9C1F-5FE4264B61BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32760" yWindow="460" windowWidth="32780" windowHeight="20540" xr2:uid="{592E1224-DF50-6D4D-B05A-DA289C9EE1FD}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="32780" windowHeight="20540" xr2:uid="{592E1224-DF50-6D4D-B05A-DA289C9EE1FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$12</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Definition</t>
   </si>
@@ -218,6 +221,43 @@
   </si>
   <si>
     <t>Chi-Square distribution</t>
+  </si>
+  <si>
+    <t>np</t>
+  </si>
+  <si>
+    <t>np(1-p)</t>
+  </si>
+  <si>
+    <t>(a+b)/2</t>
+  </si>
+  <si>
+    <t>(b-a)^2 / 12</t>
+  </si>
+  <si>
+    <t>μ</t>
+  </si>
+  <si>
+    <t>σ^2</t>
+  </si>
+  <si>
+    <t>PDF/PMF</t>
+  </si>
+  <si>
+    <t>p, if x = 1
+1-p, if x = 0</t>
+  </si>
+  <si>
+    <t>nCk p^k (1-p)^n-k for k = 0, 1, 2.., n</t>
+  </si>
+  <si>
+    <t>p(1-p)^k-1 for k = 1, 2, ..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(e^-ƛ * ƛ^k) / k! </t>
+  </si>
+  <si>
+    <t>1/(b-a) for all x belonging to (a,b)</t>
   </si>
 </sst>
 </file>
@@ -293,6 +333,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16933</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3605102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1549400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3810000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DF5E50F-1267-7E46-B13F-C6AF529A9D32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5410200" y="15712435"/>
+          <a:ext cx="1532467" cy="204898"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,34 +681,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884D6EF3-0CDC-5F48-BA57-5033236E4292}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="17">
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="17">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -629,23 +718,26 @@
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="68">
+    <row r="3" spans="1:9" ht="68">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -655,20 +747,23 @@
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="136">
+    <row r="4" spans="1:9" ht="136">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -678,11 +773,20 @@
       <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
       <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="102">
+    <row r="5" spans="1:9" ht="102">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -693,7 +797,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="409.6">
+    <row r="6" spans="1:9" ht="409.6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -703,23 +807,26 @@
       <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
+      <c r="D6" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="204">
+    <row r="7" spans="1:9" ht="204">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -729,21 +836,24 @@
       <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="306">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="306">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -753,14 +863,20 @@
       <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F8">
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="153">
+    <row r="9" spans="1:9" ht="153">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -770,12 +886,21 @@
       <c r="C9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9">
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="238">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="238">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -785,14 +910,14 @@
       <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="68">
+    <row r="11" spans="1:9" ht="68">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -802,11 +927,11 @@
       <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="102">
+    <row r="12" spans="1:9" ht="102">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -816,14 +941,16 @@
       <c r="C12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add examples to a couple of distributions
</commit_message>
<xml_diff>
--- a/probability_distributions_cheat_sheet.xlsx
+++ b/probability_distributions_cheat_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syerrapr/Documents/personal/cheat-sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C824AD07-BA0A-5343-9C1F-5FE4264B61BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13982EEA-6E17-2E41-95A3-CD5CE6F717A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="460" windowWidth="32780" windowHeight="20540" xr2:uid="{592E1224-DF50-6D4D-B05A-DA289C9EE1FD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>Definition</t>
   </si>
@@ -169,11 +169,6 @@
     <t>Averages of samples of observations of random variables independently drawn from independent distributions converge in distribution to the normal, that is, they become normally distributed when the number of observations is sufficiently large.</t>
   </si>
   <si>
-    <t xml:space="preserve">Normal distributions are important in statistics and are often used in the natural and social sciences to represent real-valued random variables whose distributions are not known.
-Physical quantities that are expected to be the sum of many independent processes (such as measurement errors) often have distributions that are nearly normal.
-Moreover, many results and methods (such as propagation of uncertainty and least squares parameter fitting) can be derived analytically in explicit form when the relevant variables are normally distributed. </t>
-  </si>
-  <si>
     <t>Uniform distribution
 (Rectangular distribution)</t>
   </si>
@@ -258,6 +253,15 @@
   </si>
   <si>
     <t>1/(b-a) for all x belonging to (a,b)</t>
+  </si>
+  <si>
+    <t>No. of heads when we toss a coin 20 times</t>
+  </si>
+  <si>
+    <t>Normal distributions are important in statistics and are often used in the natural and social sciences to represent real-valued random variables whose distributions are not known.
+Physical quantities that are expected to be the sum of many independent processes (such as measurement errors) often have distributions that are nearly normal.
+Moreover, many results and methods (such as propagation of uncertainty and least squares parameter fitting) can be derived analytically in explicit form when the relevant variables are normally distributed. 
+Thermal noise in communication systems</t>
   </si>
 </sst>
 </file>
@@ -683,7 +687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884D6EF3-0CDC-5F48-BA57-5033236E4292}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -719,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -734,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="68">
@@ -748,7 +754,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -774,16 +780,19 @@
         <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
         <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="102">
@@ -808,7 +817,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -837,7 +846,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -853,7 +862,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="306">
+    <row r="8" spans="1:9" ht="356">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -864,36 +873,36 @@
         <v>34</v>
       </c>
       <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
         <v>52</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="153">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -902,47 +911,47 @@
     </row>
     <row r="10" spans="1:9" ht="238">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="68">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="102">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>